<commit_message>
pengeluaran + pengadaan error terus
</commit_message>
<xml_diff>
--- a/public/files/template/inventory/lap_bhp_ketersediaan.xlsx
+++ b/public/files/template/inventory/lap_bhp_ketersediaan.xlsx
@@ -191,9 +191,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -206,6 +203,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -514,7 +514,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,22 +527,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -573,82 +573,82 @@
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>1</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>2</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>4</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>5</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>